<commit_message>
List of all Commands used in this Course
</commit_message>
<xml_diff>
--- a/Kubernetes-Commands.xlsx
+++ b/Kubernetes-Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\A-K8S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\K8S - Kubernetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9B2D73-91C1-4D87-BD1A-4D22B5BF9440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3260E202-2187-47A0-970F-D0D63BCDAA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD72DAEC-706C-4818-B11F-A045285E270B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FD72DAEC-706C-4818-B11F-A045285E270B}"/>
   </bookViews>
   <sheets>
     <sheet name="K8s Commands" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="163">
   <si>
     <t>minikube start</t>
   </si>
@@ -496,12 +490,99 @@
   <si>
     <t>Course by Denis Astahov</t>
   </si>
+  <si>
+    <t>kubectl apply -f https://projectcontour.io/quickstart/contour.yaml</t>
+  </si>
+  <si>
+    <t>Создать Ingress Controller Contour</t>
+  </si>
+  <si>
+    <t>kubectl get services -n projectcontour envoy -o wide</t>
+  </si>
+  <si>
+    <t>Показать Ingess Controller Load Balancer данные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kubectl create deployment main    --image=adv4000/k8sphp:latest </t>
+  </si>
+  <si>
+    <t>kubectl create deployment web1    --image=adv4000/k8sphp:version1</t>
+  </si>
+  <si>
+    <t>kubectl create deployment web2    --image=adv4000/k8sphp:version2</t>
+  </si>
+  <si>
+    <t>kubectl scale deployment main    --replicas 2</t>
+  </si>
+  <si>
+    <t>kubectl scale deployment web1    --replicas 2</t>
+  </si>
+  <si>
+    <t>kubectl scale deployment web2    --replicas 2</t>
+  </si>
+  <si>
+    <t>kubectl expose deployment main   --port 80   # --type=ClusterIP  DEFAULT</t>
+  </si>
+  <si>
+    <t>kubectl expose deployment web1   --port 80</t>
+  </si>
+  <si>
+    <t>kubectl expose deployment web2   --port 80</t>
+  </si>
+  <si>
+    <t>kubectl expose deployment tomcat --port 8080</t>
+  </si>
+  <si>
+    <t>kubectl get services -o wide</t>
+  </si>
+  <si>
+    <t>kubectl get ingress</t>
+  </si>
+  <si>
+    <t>kubectl describe ingress</t>
+  </si>
+  <si>
+    <t>kubectl delete ns projectcontour</t>
+  </si>
+  <si>
+    <t>Создать Deployment</t>
+  </si>
+  <si>
+    <t>Создать Service, по умолчанию тип ClusterIP</t>
+  </si>
+  <si>
+    <t>Показать данные всех Services</t>
+  </si>
+  <si>
+    <t>kubectl apply -f ingress-hosts.yaml</t>
+  </si>
+  <si>
+    <t>kubectl apply -f ingress-paths.yaml</t>
+  </si>
+  <si>
+    <t>Создать Ingress Rules из файла</t>
+  </si>
+  <si>
+    <t>Показать все созданные Ingress Rules</t>
+  </si>
+  <si>
+    <t>Показать все созданные Ingress Rules подробно</t>
+  </si>
+  <si>
+    <t>Стереть полностью Ingress Controller Contour</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/191WWNpjJ2za6-nbG4ZoUMXMpUK8KlCIosvQB0f-oq3k/</t>
+  </si>
+  <si>
+    <t>Comparison of Ingress Controllers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +627,21 @@
     </font>
     <font>
       <sz val="48"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -640,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -651,6 +747,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,16 +1066,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC433D39-1F4B-4563-8B50-9BB3F575A520}">
-  <dimension ref="B1:C128"/>
+  <dimension ref="B1:C157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="131.6640625" customWidth="1"/>
-    <col min="3" max="3" width="111.44140625" customWidth="1"/>
+    <col min="2" max="2" width="123.6640625" customWidth="1"/>
+    <col min="3" max="3" width="88.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="61.2" x14ac:dyDescent="1.1000000000000001">
@@ -1723,6 +1824,177 @@
         <v>131</v>
       </c>
     </row>
+    <row r="130" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="131" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B131" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B132" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B133" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B134" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B135" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B136" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B137" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B138" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B139" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B140" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C140" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B141" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B142" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C142" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B143" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C143" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B144" s="3"/>
+      <c r="C144" s="11"/>
+    </row>
+    <row r="145" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B145" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C145" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B146" s="3"/>
+      <c r="C146" s="11"/>
+    </row>
+    <row r="147" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B147" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C147" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B148" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C148" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B149" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C149" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B150" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C150" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B151" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C151" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B156" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B157" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>